<commit_message>
completed figures for evaluatie gp2018
</commit_message>
<xml_diff>
--- a/output/tabellen_evaluatie_gj2018.xlsx
+++ b/output/tabellen_evaluatie_gj2018.xlsx
@@ -15,59 +15,6 @@
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
-  <si>
-    <t>prognose</t>
-  </si>
-  <si>
-    <t>realisatie</t>
-  </si>
-  <si>
-    <t>landingen</t>
-  </si>
-  <si>
-    <t>starts</t>
-  </si>
-  <si>
-    <t>totaal</t>
-  </si>
-  <si>
-    <t>dag 07-19 uur</t>
-  </si>
-  <si>
-    <t>avond 19-23 uur</t>
-  </si>
-  <si>
-    <t>nacht 23-06 uur</t>
-  </si>
-  <si>
-    <t>vroege ochtend 06-07 uur</t>
-  </si>
-  <si>
-    <t>winter</t>
-  </si>
-  <si>
-    <t>zomer</t>
-  </si>
-  <si>
-    <t>NADP1</t>
-  </si>
-  <si>
-    <t>NADP2</t>
-  </si>
-  <si>
-    <t>2000 [ft]</t>
-  </si>
-  <si>
-    <t>3000 [ft]</t>
-  </si>
-  <si>
-    <t>CDA</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -93,7 +40,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -103,6 +50,34 @@
     </border>
     <border>
       <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
@@ -422,43 +397,61 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="1" t="s"/>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr"/>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>prognose</t>
+        </is>
       </c>
       <c r="C1" s="1" t="n"/>
       <c r="D1" s="1" t="n"/>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>realisatie</t>
+        </is>
       </c>
       <c r="F1" s="1" t="n"/>
       <c r="G1" s="1" t="n"/>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="1" t="s"/>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr"/>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>landingen</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>starts</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>totaal</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>landingen</t>
+        </is>
+      </c>
+      <c r="F2" s="1" t="inlineStr">
+        <is>
+          <t>starts</t>
+        </is>
+      </c>
+      <c r="G2" s="1" t="inlineStr">
+        <is>
+          <t>totaal</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>dag 07-19 uur</t>
+        </is>
       </c>
       <c r="B4" t="n">
         <v>172500</v>
@@ -479,9 +472,11 @@
         <v>359800</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>avond 19-23 uur</t>
+        </is>
       </c>
       <c r="B5" t="n">
         <v>53600</v>
@@ -502,9 +497,11 @@
         <v>106400</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>nacht 23-06 uur</t>
+        </is>
       </c>
       <c r="B6" t="n">
         <v>12300</v>
@@ -525,9 +522,11 @@
         <v>20200</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>vroege ochtend 06-07 uur</t>
+        </is>
       </c>
       <c r="B7" t="n">
         <v>9500</v>
@@ -548,9 +547,11 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="1" t="s">
-        <v>4</v>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>totaal</t>
+        </is>
       </c>
       <c r="B8" t="n">
         <v>248000</v>
@@ -594,17 +595,23 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
-        <v>9</v>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>prognose</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>realisatie</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>winter</t>
+        </is>
       </c>
       <c r="B2" t="n">
         <v>179300</v>
@@ -613,9 +620,11 @@
         <v>177300</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1" t="s">
-        <v>10</v>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>zomer</t>
+        </is>
       </c>
       <c r="B3" t="n">
         <v>317200</v>
@@ -643,17 +652,23 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
-        <v>11</v>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>prognose</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>realisatie</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>NADP1</t>
+        </is>
       </c>
       <c r="B2" t="n">
         <v>20.3</v>
@@ -662,9 +677,11 @@
         <v>18.4</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1" t="s">
-        <v>12</v>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>NADP2</t>
+        </is>
       </c>
       <c r="B3" t="n">
         <v>79.7</v>
@@ -692,17 +709,23 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
-        <v>13</v>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>prognose</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>realisatie</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>2000 [ft]</t>
+        </is>
       </c>
       <c r="B2" t="n">
         <v>47.3</v>
@@ -711,9 +734,11 @@
         <v>43.6</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1" t="s">
-        <v>14</v>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>3000 [ft]</t>
+        </is>
       </c>
       <c r="B3" t="n">
         <v>19.1</v>
@@ -722,9 +747,11 @@
         <v>18.9</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1" t="s">
-        <v>15</v>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>CDA</t>
+        </is>
       </c>
       <c r="B4" t="n">
         <v>33.6</v>

</xml_diff>